<commit_message>
Fix treatment input issue
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-Carma-CCS.xlsx
+++ b/premise/data/additional_inventories/lci-Carma-CCS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4E3095-55FC-C147-9E6D-0D1D87E780FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F7108A-4222-A543-82E1-59A6DED617BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2932,7 +2932,7 @@
   <dimension ref="A1:O2630"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2638" sqref="A2638"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18015,12 +18015,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="730" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="730" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A730" t="s">
         <v>191</v>
       </c>
       <c r="B730">
-        <v>-505000</v>
+        <v>505000</v>
       </c>
       <c r="C730" t="s">
         <v>4</v>
@@ -18050,12 +18050,12 @@
         <v>476</v>
       </c>
     </row>
-    <row r="731" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="731" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A731" t="s">
         <v>193</v>
       </c>
       <c r="B731">
-        <v>-252000</v>
+        <v>252000</v>
       </c>
       <c r="C731" t="s">
         <v>4</v>
@@ -22308,12 +22308,12 @@
         <v>689</v>
       </c>
     </row>
-    <row r="870" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="870" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A870" t="s">
         <v>191</v>
       </c>
       <c r="B870">
-        <v>-3.1349999999999999E-8</v>
+        <v>3.1349999999999999E-8</v>
       </c>
       <c r="C870" t="s">
         <v>4</v>
@@ -22343,12 +22343,12 @@
         <v>690</v>
       </c>
     </row>
-    <row r="871" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="871" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A871" t="s">
         <v>193</v>
       </c>
       <c r="B871">
-        <v>-1.5675E-8</v>
+        <v>1.5675E-8</v>
       </c>
       <c r="C871" t="s">
         <v>4</v>
@@ -31019,12 +31019,12 @@
         <v>624</v>
       </c>
     </row>
-    <row r="1152" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1152" t="s">
         <v>191</v>
       </c>
       <c r="B1152">
-        <v>-3.1349999999999999E-8</v>
+        <v>3.1349999999999999E-8</v>
       </c>
       <c r="C1152" t="s">
         <v>4</v>
@@ -31051,12 +31051,12 @@
         <v>476</v>
       </c>
     </row>
-    <row r="1153" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1153" t="s">
         <v>193</v>
       </c>
       <c r="B1153">
-        <v>-1.5675E-8</v>
+        <v>1.5675E-8</v>
       </c>
       <c r="C1153" t="s">
         <v>4</v>
@@ -50368,7 +50368,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="1826" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1826" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1826" t="s">
         <v>511</v>
       </c>
@@ -52653,7 +52653,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="1898" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1898" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1898" t="s">
         <v>511</v>
       </c>
@@ -63047,12 +63047,12 @@
         <v>624</v>
       </c>
     </row>
-    <row r="2319" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2319" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2319" t="s">
         <v>191</v>
       </c>
       <c r="B2319">
-        <v>-505000</v>
+        <v>505000</v>
       </c>
       <c r="C2319" t="s">
         <v>4</v>
@@ -63085,12 +63085,12 @@
         <v>476</v>
       </c>
     </row>
-    <row r="2320" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2320" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2320" t="s">
         <v>193</v>
       </c>
       <c r="B2320">
-        <v>-252000</v>
+        <v>252000</v>
       </c>
       <c r="C2320" t="s">
         <v>4</v>
@@ -71862,7 +71862,8 @@
   <autoFilter ref="A1:N2630" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="treatment of wastewater, average, capacity 1.1E10l/year"/>
+        <filter val="treatment of aluminium scrap, new, at refiner"/>
+        <filter val="treatment of aluminium scrap, post-consumer, prepared for recycling, at refiner"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>